<commit_message>
fixed missing data in health faci for linked bars
</commit_message>
<xml_diff>
--- a/data101_data/response_per_reg.xlsx
+++ b/data101_data/response_per_reg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JUPYTER FILES\DATA101\Project\Final Project Dash App\D101_Interactive_Visualization_Project\data101_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D26A3D-2C26-4FC3-A517-EEC71F51EE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6CD571-39C2-4B5B-87E3-37B7CD40EEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="109">
   <si>
     <t>Province</t>
   </si>
@@ -323,6 +323,30 @@
   </si>
   <si>
     <t>MIMAROPA REGION</t>
+  </si>
+  <si>
+    <t>CITY OF ISABELA (NOT A PROVINCE)</t>
+  </si>
+  <si>
+    <t>COMPOSTELA VALLEY</t>
+  </si>
+  <si>
+    <t>COTABATO CITY (NOT A PROVINCE)</t>
+  </si>
+  <si>
+    <t>NCR, CITY OF MANILA, FIRST DISTRICT (NOT A PROVINCE)</t>
+  </si>
+  <si>
+    <t>NATIONAL CAPITAL REGION (NCR)</t>
+  </si>
+  <si>
+    <t>NCR, FOURTH DISTRICT (NOT A PROVINCE)</t>
+  </si>
+  <si>
+    <t>NCR, SECOND DISTRICT (NOT A PROVINCE)</t>
+  </si>
+  <si>
+    <t>NCR, THIRD DISTRICT (NOT A PROVINCE)</t>
   </si>
 </sst>
 </file>
@@ -688,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E81"/>
+      <selection sqref="A1:E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1140,936 +1164,1055 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C27">
-        <v>305</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>587</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>910</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="B28" t="s">
         <v>35</v>
       </c>
       <c r="C28">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="D28">
-        <v>315</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>425</v>
+        <v>404</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="C29">
-        <v>249</v>
+        <v>305</v>
       </c>
       <c r="D29">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="E29">
-        <v>664</v>
+        <v>910</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>103</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="C30">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="D30">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>189</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
         <v>35</v>
       </c>
       <c r="C31">
-        <v>66</v>
+        <v>149</v>
       </c>
       <c r="D31">
-        <v>218</v>
+        <v>315</v>
       </c>
       <c r="E31">
-        <v>383</v>
+        <v>425</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C32">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="D32">
-        <v>36</v>
+        <v>595</v>
       </c>
       <c r="E32">
-        <v>139</v>
+        <v>664</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C33">
-        <v>125</v>
+        <v>39</v>
       </c>
       <c r="D33">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="E33">
-        <v>529</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="C34">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="D34">
-        <v>95</v>
+        <v>218</v>
       </c>
       <c r="E34">
-        <v>114</v>
+        <v>383</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C35">
-        <v>197</v>
+        <v>234</v>
       </c>
       <c r="D35">
-        <v>212</v>
+        <v>36</v>
       </c>
       <c r="E35">
-        <v>263</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C36">
-        <v>273</v>
+        <v>125</v>
       </c>
       <c r="D36">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="E36">
-        <v>443</v>
+        <v>529</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="C37">
-        <v>294</v>
+        <v>47</v>
       </c>
       <c r="D37">
-        <v>503</v>
+        <v>95</v>
       </c>
       <c r="E37">
-        <v>567</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C38">
-        <v>386</v>
+        <v>197</v>
       </c>
       <c r="D38">
-        <v>660</v>
+        <v>212</v>
       </c>
       <c r="E38">
-        <v>1279</v>
+        <v>263</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C39">
-        <v>468</v>
+        <v>273</v>
       </c>
       <c r="D39">
-        <v>964</v>
+        <v>181</v>
       </c>
       <c r="E39">
-        <v>1143</v>
+        <v>443</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="C40">
-        <v>179</v>
+        <v>294</v>
       </c>
       <c r="D40">
-        <v>158</v>
+        <v>503</v>
       </c>
       <c r="E40">
-        <v>292</v>
+        <v>567</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="C41">
-        <v>216</v>
+        <v>386</v>
       </c>
       <c r="D41">
-        <v>346</v>
+        <v>660</v>
       </c>
       <c r="E41">
-        <v>441</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="C42">
-        <v>486</v>
+        <v>468</v>
       </c>
       <c r="D42">
-        <v>610</v>
+        <v>964</v>
       </c>
       <c r="E42">
-        <v>591</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C43">
-        <v>137</v>
+        <v>179</v>
       </c>
       <c r="D43">
-        <v>303</v>
+        <v>158</v>
       </c>
       <c r="E43">
-        <v>489</v>
+        <v>292</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>216</v>
       </c>
       <c r="D44">
-        <v>242</v>
+        <v>346</v>
       </c>
       <c r="E44">
-        <v>879</v>
+        <v>441</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="C45">
-        <v>11</v>
+        <v>486</v>
       </c>
       <c r="D45">
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="E45">
-        <v>1500</v>
+        <v>591</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>137</v>
       </c>
       <c r="D46">
-        <v>344</v>
+        <v>303</v>
       </c>
       <c r="E46">
-        <v>633</v>
+        <v>489</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C47">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>48</v>
+        <v>242</v>
       </c>
       <c r="E47">
-        <v>228</v>
+        <v>879</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C48">
-        <v>202</v>
+        <v>11</v>
       </c>
       <c r="D48">
-        <v>383</v>
+        <v>605</v>
       </c>
       <c r="E48">
-        <v>737</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C49">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>183</v>
+        <v>344</v>
       </c>
       <c r="E49">
-        <v>531</v>
+        <v>633</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="C50">
-        <v>171</v>
+        <v>119</v>
       </c>
       <c r="D50">
-        <v>519</v>
+        <v>48</v>
       </c>
       <c r="E50">
-        <v>651</v>
+        <v>228</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C51">
-        <v>85</v>
+        <v>202</v>
       </c>
       <c r="D51">
-        <v>149</v>
+        <v>383</v>
       </c>
       <c r="E51">
-        <v>264</v>
+        <v>737</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C52">
-        <v>574</v>
+        <v>95</v>
       </c>
       <c r="D52">
-        <v>764</v>
+        <v>183</v>
       </c>
       <c r="E52">
-        <v>1207</v>
+        <v>531</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B53" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C53">
-        <v>290</v>
+        <v>171</v>
       </c>
       <c r="D53">
-        <v>552</v>
+        <v>519</v>
       </c>
       <c r="E53">
-        <v>894</v>
+        <v>651</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C54">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="D54">
-        <v>231</v>
+        <v>149</v>
       </c>
       <c r="E54">
-        <v>603</v>
+        <v>264</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="C55">
-        <v>278</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>511</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>935</v>
+        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="B56" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="C56">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="D56">
-        <v>268</v>
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>379</v>
+        <v>217</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="B57" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C57">
-        <v>84</v>
+        <v>139</v>
       </c>
       <c r="D57">
-        <v>151</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>348</v>
+        <v>255</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="B58" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C58">
-        <v>579</v>
+        <v>95</v>
       </c>
       <c r="D58">
-        <v>465</v>
+        <v>0</v>
       </c>
       <c r="E58">
-        <v>566</v>
+        <v>206</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="C59">
-        <v>401</v>
+        <v>574</v>
       </c>
       <c r="D59">
-        <v>430</v>
+        <v>764</v>
       </c>
       <c r="E59">
-        <v>875</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C60">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="D60">
-        <v>650</v>
+        <v>552</v>
       </c>
       <c r="E60">
-        <v>727</v>
+        <v>894</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C61">
-        <v>387</v>
+        <v>109</v>
       </c>
       <c r="D61">
-        <v>1195</v>
+        <v>231</v>
       </c>
       <c r="E61">
-        <v>1505</v>
+        <v>603</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="C62">
-        <v>911</v>
+        <v>278</v>
       </c>
       <c r="D62">
-        <v>869</v>
+        <v>511</v>
       </c>
       <c r="E62">
-        <v>1047</v>
+        <v>935</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>27</v>
       </c>
       <c r="C63">
-        <v>25</v>
+        <v>231</v>
       </c>
       <c r="D63">
-        <v>159</v>
+        <v>268</v>
       </c>
       <c r="E63">
-        <v>211</v>
+        <v>379</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C64">
-        <v>331</v>
+        <v>84</v>
       </c>
       <c r="D64">
-        <v>398</v>
+        <v>151</v>
       </c>
       <c r="E64">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>100</v>
       </c>
       <c r="C65">
-        <v>289</v>
+        <v>579</v>
       </c>
       <c r="D65">
-        <v>221</v>
+        <v>465</v>
       </c>
       <c r="E65">
-        <v>260</v>
+        <v>566</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C66">
-        <v>100</v>
+        <v>401</v>
       </c>
       <c r="D66">
-        <v>253</v>
+        <v>430</v>
       </c>
       <c r="E66">
-        <v>983</v>
+        <v>875</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="C67">
-        <v>150</v>
+        <v>286</v>
       </c>
       <c r="D67">
-        <v>170</v>
+        <v>650</v>
       </c>
       <c r="E67">
-        <v>405</v>
+        <v>727</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C68">
-        <v>94</v>
+        <v>387</v>
       </c>
       <c r="D68">
-        <v>67</v>
+        <v>1195</v>
       </c>
       <c r="E68">
-        <v>79</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="C69">
-        <v>185</v>
+        <v>911</v>
       </c>
       <c r="D69">
-        <v>450</v>
+        <v>869</v>
       </c>
       <c r="E69">
-        <v>615</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>95</v>
+        <v>27</v>
       </c>
       <c r="C70">
-        <v>390</v>
+        <v>25</v>
       </c>
       <c r="D70">
-        <v>369</v>
+        <v>159</v>
       </c>
       <c r="E70">
-        <v>543</v>
+        <v>211</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="C71">
-        <v>525</v>
+        <v>331</v>
       </c>
       <c r="D71">
-        <v>175</v>
+        <v>398</v>
       </c>
       <c r="E71">
-        <v>418</v>
+        <v>353</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C72">
-        <v>81</v>
+        <v>289</v>
       </c>
       <c r="D72">
-        <v>302</v>
+        <v>221</v>
       </c>
       <c r="E72">
-        <v>442</v>
+        <v>260</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D73">
-        <v>171</v>
+        <v>253</v>
       </c>
       <c r="E73">
-        <v>456</v>
+        <v>983</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="C74">
-        <v>224</v>
+        <v>150</v>
       </c>
       <c r="D74">
-        <v>201</v>
+        <v>170</v>
       </c>
       <c r="E74">
-        <v>428</v>
+        <v>405</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C75">
-        <v>362</v>
+        <v>94</v>
       </c>
       <c r="D75">
-        <v>313</v>
+        <v>67</v>
       </c>
       <c r="E75">
-        <v>570</v>
+        <v>79</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C76">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D76">
-        <v>309</v>
+        <v>450</v>
       </c>
       <c r="E76">
-        <v>599</v>
+        <v>615</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="D77">
-        <v>103</v>
+        <v>369</v>
       </c>
       <c r="E77">
-        <v>262</v>
+        <v>543</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C78">
-        <v>124</v>
+        <v>525</v>
       </c>
       <c r="D78">
-        <v>274</v>
+        <v>175</v>
       </c>
       <c r="E78">
-        <v>368</v>
+        <v>418</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C79">
-        <v>178</v>
+        <v>81</v>
       </c>
       <c r="D79">
-        <v>431</v>
+        <v>302</v>
       </c>
       <c r="E79">
-        <v>865</v>
+        <v>442</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="C80">
-        <v>293</v>
+        <v>0</v>
       </c>
       <c r="D80">
-        <v>434</v>
+        <v>171</v>
       </c>
       <c r="E80">
-        <v>1097</v>
+        <v>456</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81">
+        <v>224</v>
+      </c>
+      <c r="D81">
+        <v>201</v>
+      </c>
+      <c r="E81">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82">
+        <v>362</v>
+      </c>
+      <c r="D82">
+        <v>313</v>
+      </c>
+      <c r="E82">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>17</v>
+      </c>
+      <c r="C83">
+        <v>194</v>
+      </c>
+      <c r="D83">
+        <v>309</v>
+      </c>
+      <c r="E83">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>50</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>103</v>
+      </c>
+      <c r="E84">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>17</v>
+      </c>
+      <c r="C85">
+        <v>124</v>
+      </c>
+      <c r="D85">
+        <v>274</v>
+      </c>
+      <c r="E85">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>86</v>
+      </c>
+      <c r="C86">
+        <v>178</v>
+      </c>
+      <c r="D86">
+        <v>431</v>
+      </c>
+      <c r="E86">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>87</v>
+      </c>
+      <c r="B87" t="s">
+        <v>86</v>
+      </c>
+      <c r="C87">
+        <v>293</v>
+      </c>
+      <c r="D87">
+        <v>434</v>
+      </c>
+      <c r="E87">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>88</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B88" t="s">
         <v>86</v>
       </c>
-      <c r="C81">
+      <c r="C88">
         <v>124</v>
       </c>
-      <c r="D81">
+      <c r="D88">
         <v>170</v>
       </c>
-      <c r="E81">
+      <c r="E88">
         <v>506</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated image and font sizes for single values
</commit_message>
<xml_diff>
--- a/data101_data/response_per_reg.xlsx
+++ b/data101_data/response_per_reg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JUPYTER FILES\DATA101\Project\Final Project Dash App\D101_Interactive_Visualization_Project\data101_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6CD571-39C2-4B5B-87E3-37B7CD40EEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB04F09E-9BCB-4CE7-8B1A-2AA441ADE37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,15 +28,6 @@
     <t>Region</t>
   </si>
   <si>
-    <t>T_Evacuation</t>
-  </si>
-  <si>
-    <t>T_Health</t>
-  </si>
-  <si>
-    <t>T_School</t>
-  </si>
-  <si>
     <t>ABRA</t>
   </si>
   <si>
@@ -347,6 +338,15 @@
   </si>
   <si>
     <t>NCR, THIRD DISTRICT (NOT A PROVINCE)</t>
+  </si>
+  <si>
+    <t>Evacuation Centers</t>
+  </si>
+  <si>
+    <t>Health Facilities</t>
+  </si>
+  <si>
+    <t>Schools</t>
   </si>
 </sst>
 </file>
@@ -715,7 +715,7 @@
   <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E88"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,21 +728,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>106</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>265</v>
@@ -756,10 +756,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>215</v>
@@ -773,10 +773,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>127</v>
@@ -790,10 +790,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>167</v>
@@ -807,10 +807,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>350</v>
@@ -824,10 +824,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>239</v>
@@ -841,10 +841,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>148</v>
@@ -858,10 +858,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>347</v>
@@ -875,10 +875,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -892,10 +892,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>55</v>
@@ -909,10 +909,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C12">
         <v>26</v>
@@ -926,10 +926,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C13">
         <v>485</v>
@@ -943,10 +943,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>461</v>
@@ -960,10 +960,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C15">
         <v>144</v>
@@ -977,10 +977,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C16">
         <v>741</v>
@@ -994,10 +994,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C17">
         <v>174</v>
@@ -1011,10 +1011,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>278</v>
@@ -1028,10 +1028,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C19">
         <v>203</v>
@@ -1045,10 +1045,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C20">
         <v>524</v>
@@ -1062,10 +1062,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C21">
         <v>415</v>
@@ -1079,10 +1079,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>108</v>
@@ -1096,10 +1096,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C23">
         <v>377</v>
@@ -1113,10 +1113,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C24">
         <v>6</v>
@@ -1130,10 +1130,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C25">
         <v>454</v>
@@ -1147,10 +1147,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C26">
         <v>694</v>
@@ -1164,10 +1164,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1181,10 +1181,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C28">
         <v>185</v>
@@ -1198,10 +1198,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C29">
         <v>305</v>
@@ -1215,10 +1215,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -1232,10 +1232,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C31">
         <v>149</v>
@@ -1249,10 +1249,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>249</v>
@@ -1266,10 +1266,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>39</v>
@@ -1283,10 +1283,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C34">
         <v>66</v>
@@ -1300,10 +1300,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C35">
         <v>234</v>
@@ -1317,10 +1317,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C36">
         <v>125</v>
@@ -1334,10 +1334,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B37" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C37">
         <v>47</v>
@@ -1351,10 +1351,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C38">
         <v>197</v>
@@ -1368,10 +1368,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C39">
         <v>273</v>
@@ -1385,10 +1385,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C40">
         <v>294</v>
@@ -1402,10 +1402,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C41">
         <v>386</v>
@@ -1419,10 +1419,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C42">
         <v>468</v>
@@ -1436,10 +1436,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C43">
         <v>179</v>
@@ -1453,10 +1453,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C44">
         <v>216</v>
@@ -1470,10 +1470,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C45">
         <v>486</v>
@@ -1487,10 +1487,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C46">
         <v>137</v>
@@ -1504,10 +1504,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1521,10 +1521,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C48">
         <v>11</v>
@@ -1538,10 +1538,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -1555,10 +1555,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C50">
         <v>119</v>
@@ -1572,10 +1572,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C51">
         <v>202</v>
@@ -1589,10 +1589,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C52">
         <v>95</v>
@@ -1606,10 +1606,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C53">
         <v>171</v>
@@ -1623,10 +1623,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C54">
         <v>85</v>
@@ -1640,10 +1640,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B55" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -1657,10 +1657,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B56" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C56">
         <v>212</v>
@@ -1674,10 +1674,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B57" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C57">
         <v>139</v>
@@ -1691,10 +1691,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B58" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C58">
         <v>95</v>
@@ -1708,10 +1708,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B59" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C59">
         <v>574</v>
@@ -1725,10 +1725,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B60" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C60">
         <v>290</v>
@@ -1742,10 +1742,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C61">
         <v>109</v>
@@ -1759,10 +1759,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C62">
         <v>278</v>
@@ -1776,10 +1776,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B63" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C63">
         <v>231</v>
@@ -1793,10 +1793,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B64" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C64">
         <v>84</v>
@@ -1810,10 +1810,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B65" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C65">
         <v>579</v>
@@ -1827,10 +1827,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B66" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C66">
         <v>401</v>
@@ -1844,10 +1844,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B67" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C67">
         <v>286</v>
@@ -1861,10 +1861,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B68" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C68">
         <v>387</v>
@@ -1878,10 +1878,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B69" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C69">
         <v>911</v>
@@ -1895,10 +1895,10 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B70" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C70">
         <v>25</v>
@@ -1912,10 +1912,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B71" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C71">
         <v>331</v>
@@ -1929,10 +1929,10 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B72" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C72">
         <v>289</v>
@@ -1946,10 +1946,10 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B73" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C73">
         <v>100</v>
@@ -1963,10 +1963,10 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B74" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C74">
         <v>150</v>
@@ -1980,10 +1980,10 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B75" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C75">
         <v>94</v>
@@ -1997,10 +1997,10 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B76" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C76">
         <v>185</v>
@@ -2014,10 +2014,10 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B77" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C77">
         <v>390</v>
@@ -2031,10 +2031,10 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B78" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C78">
         <v>525</v>
@@ -2048,10 +2048,10 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B79" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C79">
         <v>81</v>
@@ -2065,10 +2065,10 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B80" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -2082,10 +2082,10 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B81" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C81">
         <v>224</v>
@@ -2099,10 +2099,10 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B82" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C82">
         <v>362</v>
@@ -2116,10 +2116,10 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B83" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C83">
         <v>194</v>
@@ -2133,10 +2133,10 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B84" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -2150,10 +2150,10 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B85" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C85">
         <v>124</v>
@@ -2167,10 +2167,10 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B86" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C86">
         <v>178</v>
@@ -2184,10 +2184,10 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B87" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C87">
         <v>293</v>
@@ -2201,10 +2201,10 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B88" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C88">
         <v>124</v>

</xml_diff>